<commit_message>
fix 19.10.2023 price 2h
</commit_message>
<xml_diff>
--- a/TeplosilaWeb/Content/properties/gtrv3china.xlsx
+++ b/TeplosilaWeb/Content/properties/gtrv3china.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Документы\ТЗ программа подбора TRV, RDT\ТЗ клапаны TRV\04.08.2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Документы\ТЗ программа подбора TRV, RDT\ТЗ клапаны TRV\19.10.2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -256,7 +256,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -285,15 +285,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -303,9 +294,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -323,6 +311,13 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -612,27 +607,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+    <col min="1" max="1" width="6.85546875" style="20" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" style="20" customWidth="1"/>
+    <col min="3" max="14" width="9.140625" style="20"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
     </row>
     <row r="2" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -641,20 +637,20 @@
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="15"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="12"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
@@ -780,29 +776,29 @@
       <c r="M5" s="1">
         <v>240</v>
       </c>
-      <c r="N5" s="1">
-        <v>165</v>
+      <c r="N5" s="21">
+        <v>327</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>4</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
-      <c r="K6" s="21"/>
-      <c r="L6" s="21"/>
-      <c r="M6" s="21"/>
-      <c r="N6" s="22"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="18"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
@@ -898,7 +894,7 @@
       <c r="A10" s="8">
         <v>8</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="9" t="s">
         <v>21</v>
       </c>
       <c r="C10" s="5">
@@ -925,34 +921,34 @@
       <c r="N10" s="5"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="11">
+      <c r="A11" s="8">
         <v>9</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="5">
         <v>360</v>
       </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12">
+      <c r="D11" s="5"/>
+      <c r="E11" s="5">
         <v>360</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F11" s="5">
         <v>345</v>
       </c>
-      <c r="G11" s="12">
+      <c r="G11" s="5">
         <v>350</v>
       </c>
-      <c r="H11" s="12">
+      <c r="H11" s="5">
         <v>400</v>
       </c>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="12"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
@@ -1036,7 +1032,7 @@
       <c r="A15" s="8">
         <v>13</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="9" t="s">
         <v>23</v>
       </c>
       <c r="C15" s="5"/>
@@ -1059,30 +1055,30 @@
       <c r="N15" s="5"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="11">
+      <c r="A16" s="8">
         <v>14</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12">
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5">
         <v>445</v>
       </c>
-      <c r="J16" s="12">
+      <c r="J16" s="5">
         <v>445</v>
       </c>
-      <c r="K16" s="12">
+      <c r="K16" s="5">
         <v>480</v>
       </c>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="12"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
@@ -1112,7 +1108,7 @@
       <c r="A18" s="8">
         <v>16</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="9" t="s">
         <v>25</v>
       </c>
       <c r="C18" s="5"/>
@@ -1133,28 +1129,28 @@
       <c r="N18" s="5"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="11">
+      <c r="A19" s="8">
         <v>17</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="12"/>
-      <c r="L19" s="12">
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5">
         <v>510</v>
       </c>
-      <c r="M19" s="12">
+      <c r="M19" s="5">
         <v>540</v>
       </c>
-      <c r="N19" s="12"/>
+      <c r="N19" s="5"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
@@ -1179,24 +1175,24 @@
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="11">
+      <c r="A21" s="8">
         <v>19</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="12"/>
-      <c r="L21" s="12"/>
-      <c r="M21" s="12"/>
-      <c r="N21" s="12">
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5">
         <v>555</v>
       </c>
     </row>
@@ -1316,21 +1312,21 @@
       <c r="A26" s="8">
         <v>24</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="18"/>
-      <c r="I26" s="18"/>
-      <c r="J26" s="18"/>
-      <c r="K26" s="18"/>
-      <c r="L26" s="18"/>
-      <c r="M26" s="18"/>
-      <c r="N26" s="19"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
+      <c r="K26" s="14"/>
+      <c r="L26" s="14"/>
+      <c r="M26" s="14"/>
+      <c r="N26" s="15"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
@@ -1426,7 +1422,7 @@
       <c r="A30" s="8">
         <v>28</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="9" t="s">
         <v>21</v>
       </c>
       <c r="C30" s="5">
@@ -1453,34 +1449,34 @@
       <c r="N30" s="5"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="11">
+      <c r="A31" s="8">
         <v>29</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B31" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C31" s="12">
+      <c r="C31" s="5">
         <v>5.9</v>
       </c>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12">
+      <c r="D31" s="5"/>
+      <c r="E31" s="5">
         <v>7.2</v>
       </c>
-      <c r="F31" s="12">
+      <c r="F31" s="5">
         <v>8.4</v>
       </c>
-      <c r="G31" s="12">
+      <c r="G31" s="5">
         <v>10.5</v>
       </c>
-      <c r="H31" s="12">
+      <c r="H31" s="5">
         <v>14.3</v>
       </c>
-      <c r="I31" s="12"/>
-      <c r="J31" s="12"/>
-      <c r="K31" s="12"/>
-      <c r="L31" s="12"/>
-      <c r="M31" s="12"/>
-      <c r="N31" s="12"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="5"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="8">
@@ -1564,7 +1560,7 @@
       <c r="A35" s="8">
         <v>33</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="B35" s="9" t="s">
         <v>23</v>
       </c>
       <c r="C35" s="5"/>
@@ -1587,30 +1583,30 @@
       <c r="N35" s="5"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="11">
+      <c r="A36" s="8">
         <v>34</v>
       </c>
-      <c r="B36" s="10" t="s">
+      <c r="B36" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="12"/>
-      <c r="G36" s="12"/>
-      <c r="H36" s="12"/>
-      <c r="I36" s="12">
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
+      <c r="I36" s="5">
         <v>21</v>
       </c>
-      <c r="J36" s="12">
+      <c r="J36" s="5">
         <v>25</v>
       </c>
-      <c r="K36" s="12">
+      <c r="K36" s="5">
         <v>31.3</v>
       </c>
-      <c r="L36" s="12"/>
-      <c r="M36" s="12"/>
-      <c r="N36" s="12"/>
+      <c r="L36" s="5"/>
+      <c r="M36" s="5"/>
+      <c r="N36" s="5"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="8">
@@ -1640,7 +1636,7 @@
       <c r="A38" s="8">
         <v>36</v>
       </c>
-      <c r="B38" s="10" t="s">
+      <c r="B38" s="9" t="s">
         <v>25</v>
       </c>
       <c r="C38" s="5"/>
@@ -1661,28 +1657,28 @@
       <c r="N38" s="5"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" s="11">
+      <c r="A39" s="8">
         <v>37</v>
       </c>
-      <c r="B39" s="10" t="s">
+      <c r="B39" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C39" s="12"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="12"/>
-      <c r="G39" s="12"/>
-      <c r="H39" s="12"/>
-      <c r="I39" s="12"/>
-      <c r="J39" s="12"/>
-      <c r="K39" s="12"/>
-      <c r="L39" s="12">
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="5"/>
+      <c r="K39" s="5"/>
+      <c r="L39" s="5">
         <v>39.9</v>
       </c>
-      <c r="M39" s="12">
+      <c r="M39" s="5">
         <v>56.8</v>
       </c>
-      <c r="N39" s="12"/>
+      <c r="N39" s="5"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="8">
@@ -1707,24 +1703,24 @@
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A41" s="11">
+      <c r="A41" s="8">
         <v>39</v>
       </c>
-      <c r="B41" s="10" t="s">
+      <c r="B41" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C41" s="12"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="12"/>
-      <c r="F41" s="12"/>
-      <c r="G41" s="12"/>
-      <c r="H41" s="12"/>
-      <c r="I41" s="12"/>
-      <c r="J41" s="12"/>
-      <c r="K41" s="12"/>
-      <c r="L41" s="12"/>
-      <c r="M41" s="12"/>
-      <c r="N41" s="12">
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="5"/>
+      <c r="L41" s="5"/>
+      <c r="M41" s="5"/>
+      <c r="N41" s="5">
         <v>66</v>
       </c>
     </row>

</xml_diff>